<commit_message>
add levenshtein dist option to config sheet
</commit_message>
<xml_diff>
--- a/TEMPLATE_VarRegConfig.xlsx
+++ b/TEMPLATE_VarRegConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi.bhattaraikline\Shipman_Lab_Dev\Spacer-Seq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D9B970-ABA2-4609-A4C7-1F04DBC15CE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41466819-C377-4DD4-877B-E8C7D5231EC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7070" xr2:uid="{91F791F9-F210-4310-9693-42EC842224B0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Sample</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>&lt;--- Example. Replace this row</t>
+  </si>
+  <si>
+    <t>Mismatch Tolerance (Levenshtein Distance)</t>
+  </si>
+  <si>
+    <t>Leader Proximal</t>
   </si>
 </sst>
 </file>
@@ -436,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A9427E-C949-4AC9-B9B8-611474096A09}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,7 +453,7 @@
     <col min="2" max="2" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -457,8 +463,11 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -486,8 +495,14 @@
       <c r="I2" t="s">
         <v>3</v>
       </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -515,7 +530,13 @@
       <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>